<commit_message>
Changed the path unity to EF_Unity
</commit_message>
<xml_diff>
--- a/Tools/LubanTools/DataTables/Datas/Example.xlsx
+++ b/Tools/LubanTools/DataTables/Datas/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12255"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>##var</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>10001,2;10002,12</t>
+  </si>
+  <si>
+    <t>测试</t>
+  </si>
+  <si>
+    <t>10010,7</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +1027,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="23" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="23" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1370,10 +1379,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1390,48 +1399,48 @@
     <col min="10" max="10" width="21.5" customWidth="1"/>
     <col min="11" max="11" width="31.625" customWidth="1"/>
     <col min="12" max="12" width="16.375" customWidth="1"/>
-    <col min="13" max="13" width="5.13333333333333" customWidth="1"/>
+    <col min="13" max="13" width="5.13333333333333" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
       <c r="O1"/>
       <c r="P1"/>
       <c r="Q1"/>
@@ -1455,26 +1464,26 @@
       <c r="AI1"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="7" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="9"/>
+      <c r="N2" s="10"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
@@ -1498,44 +1507,44 @@
       <c r="AI2"/>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="9"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="10"/>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
@@ -1559,32 +1568,32 @@
       <c r="AI3"/>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="9"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="10"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
@@ -1608,42 +1617,42 @@
       <c r="AI4"/>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="10" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="9"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="10"/>
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
@@ -1682,25 +1691,25 @@
       <c r="F6">
         <v>10001</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="15">
         <v>10001</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1720,25 +1729,25 @@
       <c r="F7">
         <v>10002</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>40</v>
       </c>
       <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="15">
         <v>10001</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1758,25 +1767,25 @@
       <c r="F8">
         <v>10003</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>49</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="15">
         <v>10001</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="15">
         <v>4</v>
       </c>
     </row>
@@ -1796,25 +1805,25 @@
       <c r="F9">
         <v>10004</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>49</v>
       </c>
       <c r="J9" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="15">
         <v>10001</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="15">
         <v>5</v>
       </c>
     </row>
@@ -1834,25 +1843,25 @@
       <c r="F10">
         <v>10005</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H10" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>49</v>
       </c>
       <c r="J10" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="15">
         <v>10001</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1860,7 +1869,7 @@
       <c r="B11">
         <v>10005</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D11" t="s">
@@ -1872,25 +1881,25 @@
       <c r="F11">
         <v>10006</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H11" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>65</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="15">
         <v>10001</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="15">
         <v>7</v>
       </c>
     </row>
@@ -1910,25 +1919,25 @@
       <c r="F12">
         <v>10007</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H12" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="6" t="s">
         <v>65</v>
       </c>
       <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="15">
         <v>10001</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="15">
         <v>8</v>
       </c>
     </row>
@@ -1936,10 +1945,10 @@
       <c r="B13">
         <v>10007</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>73</v>
       </c>
       <c r="E13">
@@ -1948,25 +1957,25 @@
       <c r="F13">
         <v>10008</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <v>44479.9999884259</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="J13" t="s">
         <v>74</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="15">
         <v>10001</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="15">
         <v>9</v>
       </c>
     </row>
@@ -1974,10 +1983,10 @@
       <c r="B14">
         <v>10008</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E14">
@@ -1986,25 +1995,25 @@
       <c r="F14">
         <v>10009</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="7">
         <v>44480.9999884259</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="J14" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="15">
         <v>10001</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="15">
         <v>10</v>
       </c>
     </row>
@@ -2012,10 +2021,10 @@
       <c r="B15">
         <v>10009</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E15">
@@ -2024,26 +2033,64 @@
       <c r="F15">
         <v>10000</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="6" t="s">
         <v>82</v>
       </c>
       <c r="J15" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="15">
         <v>10001</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="15">
         <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16">
+        <v>10010</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>10010</v>
+      </c>
+      <c r="G16" s="7">
+        <v>44480.9999884259</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="15">
+        <v>10001</v>
+      </c>
+      <c r="M16" s="3">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
更改Luban到1.1.1版本，新增编辑器按钮EFTools - Utility - Start Luban
</commit_message>
<xml_diff>
--- a/Tools/LubanTools/DataTables/Datas/Example.xlsx
+++ b/Tools/LubanTools/DataTables/Datas/Example.xlsx
@@ -4,30 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17655"/>
+    <workbookView windowWidth="31665" windowHeight="17670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>##var</t>
   </si>
@@ -365,11 +352,23 @@
   <si>
     <t>10010,7</t>
   </si>
+  <si>
+    <t>测试223</t>
+  </si>
+  <si>
+    <t>10011,9</t>
+  </si>
+  <si>
+    <t>测试123</t>
+  </si>
+  <si>
+    <t>121121213312</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -399,6 +398,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -412,6 +432,14 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -451,21 +479,6 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,20 +527,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -550,13 +549,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,12 +609,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -598,18 +651,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -622,36 +663,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -670,24 +687,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -701,12 +706,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,6 +782,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -811,21 +825,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -882,233 +881,231 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="22" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="23" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="23" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="22" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="22" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="23" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="23" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="23" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1379,10 +1376,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI16"/>
+  <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1706,10 +1703,10 @@
       <c r="K6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="3">
         <v>10001</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1744,10 +1741,10 @@
       <c r="K7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="3">
         <v>10001</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1782,10 +1779,10 @@
       <c r="K8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="3">
         <v>10001</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1820,10 +1817,10 @@
       <c r="K9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="3">
         <v>10001</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1858,10 +1855,10 @@
       <c r="K10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="3">
         <v>10001</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1896,10 +1893,10 @@
       <c r="K11" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="3">
         <v>10001</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="3">
         <v>7</v>
       </c>
     </row>
@@ -1934,10 +1931,10 @@
       <c r="K12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="3">
         <v>10001</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1972,10 +1969,10 @@
       <c r="K13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="3">
         <v>10001</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="3">
         <v>9</v>
       </c>
     </row>
@@ -2010,10 +2007,10 @@
       <c r="K14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="3">
         <v>10001</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="3">
         <v>10</v>
       </c>
     </row>
@@ -2048,10 +2045,10 @@
       <c r="K15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="3">
         <v>10001</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="3">
         <v>11</v>
       </c>
     </row>
@@ -2086,10 +2083,86 @@
       <c r="K16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="3">
         <v>10001</v>
       </c>
       <c r="M16" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17">
+        <v>10011</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17">
+        <v>1222</v>
+      </c>
+      <c r="F17">
+        <v>10011</v>
+      </c>
+      <c r="G17" s="7">
+        <v>45930.625</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="3">
+        <v>10001</v>
+      </c>
+      <c r="M17" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18">
+        <v>10012</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18">
+        <v>1222</v>
+      </c>
+      <c r="F18">
+        <v>10012</v>
+      </c>
+      <c r="G18" s="7">
+        <v>45930.625</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="3">
+        <v>10001</v>
+      </c>
+      <c r="M18" s="3">
         <v>12</v>
       </c>
     </row>

</xml_diff>